<commit_message>
update tidy data chapter
</commit_message>
<xml_diff>
--- a/examples/tidy-data_spreadsheets/tidy-data_comment-to-column.xlsx
+++ b/examples/tidy-data_spreadsheets/tidy-data_comment-to-column.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biodiversityaq/Desktop/data-fairy/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biodiversityaq/Desktop/data-fairy/examples/tidy-data_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C1052D-A8DE-5141-8F41-2F82B439C71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFD41F2-1FF4-9244-82AF-D750EAF08385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-29720" yWindow="2660" windowWidth="28040" windowHeight="16940" xr2:uid="{95816C59-3F9D-424D-9686-ECAB926048DB}"/>
   </bookViews>
@@ -51,10 +51,10 @@
     <t>locality</t>
   </si>
   <si>
-    <t>fieldNotes</t>
-  </si>
-  <si>
     <t>coordinates obtained from map</t>
+  </si>
+  <si>
+    <t>eventRemarks</t>
   </si>
 </sst>
 </file>
@@ -119,10 +119,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -138,10 +138,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -444,7 +440,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,28 +451,28 @@
     <col min="4" max="4" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>-62.199606666666668</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>-58.376333333333335</v>
       </c>
       <c r="D2" s="1"/>
@@ -485,10 +481,10 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>-62.203236666666669</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>-58.390805</v>
       </c>
       <c r="D3" s="1"/>
@@ -497,24 +493,24 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>-62.9</v>
       </c>
       <c r="C4" s="1">
         <v>-58.45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>-63.523561666666666</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>-60.428998333333332</v>
       </c>
       <c r="D5" s="1"/>

</xml_diff>